<commit_message>
5D log U/U doplněna rovnice aproximace
</commit_message>
<xml_diff>
--- a/Uloha5/uloha5.xlsx
+++ b/Uloha5/uloha5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vutbr-my.sharepoint.com/personal/247759_vutbr_cz/Documents/Bc. 5. Semestr/BPC-MVAA/BPC-MVAA-Protokoly-2024/Uloha5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="485" documentId="11_F25DC773A252ABDACC10484611DA68E65BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B96DF3B7-5137-4FC4-9D96-1C4C0B66EA9E}"/>
+  <xr:revisionPtr revIDLastSave="492" documentId="11_F25DC773A252ABDACC10484611DA68E65BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85419484-7619-4B01-A33F-F07C639C1931}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="30912" windowHeight="16656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5A AUDIO" sheetId="1" r:id="rId1"/>
@@ -1317,6 +1317,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1356,31 +1377,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3001,6 +3001,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0841197212683924E-2"/>
+                  <c:y val="1.5016410962653385E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="cs-CZ"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'5B'!$CM$3:$CS$3</c:f>
@@ -6231,10 +6281,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6504,15 +6550,15 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:28" ht="14.95" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:28" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6549,22 +6595,22 @@
       <c r="N3" s="2">
         <v>10</v>
       </c>
-      <c r="Q3" s="55" t="s">
+      <c r="Q3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="57"/>
-      <c r="W3" s="55" t="s">
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="46"/>
+      <c r="W3" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="57"/>
+      <c r="X3" s="45"/>
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="45"/>
+      <c r="AA3" s="45"/>
+      <c r="AB3" s="46"/>
     </row>
-    <row r="4" spans="3:28" ht="18.350000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:28" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
@@ -6613,20 +6659,20 @@
       <c r="T4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="W4" s="62" t="s">
+      <c r="W4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="X4" s="63"/>
-      <c r="Y4" s="62" t="s">
+      <c r="X4" s="48"/>
+      <c r="Y4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="Z4" s="63"/>
-      <c r="AA4" s="62" t="s">
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="AB4" s="63"/>
+      <c r="AB4" s="48"/>
     </row>
-    <row r="5" spans="3:28" ht="18.350000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:28" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
@@ -6675,20 +6721,20 @@
       <c r="T5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="W5" s="60" t="s">
+      <c r="W5" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="X5" s="61"/>
-      <c r="Y5" s="60" t="s">
+      <c r="X5" s="43"/>
+      <c r="Y5" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="Z5" s="61"/>
-      <c r="AA5" s="60" t="s">
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" s="61"/>
+      <c r="AB5" s="43"/>
     </row>
-    <row r="6" spans="3:28" ht="18.350000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:28" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
@@ -6739,21 +6785,21 @@
         <f t="array" ref="T6:T11">20*LOG((S6:S11*0.001)/(R6:R11),10)</f>
         <v>-99.901667181904344</v>
       </c>
-      <c r="W6" s="50">
+      <c r="W6" s="57">
         <v>0.29199999999999998</v>
       </c>
-      <c r="X6" s="51"/>
-      <c r="Y6" s="52">
+      <c r="X6" s="58"/>
+      <c r="Y6" s="59">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="Z6" s="51"/>
-      <c r="AA6" s="53">
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="60">
         <f>20*LOG((W6)/(Y6*0.001),10)</f>
         <v>97.2664572024091</v>
       </c>
-      <c r="AB6" s="54"/>
+      <c r="AB6" s="61"/>
     </row>
-    <row r="7" spans="3:28" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Q7" s="14">
         <v>1994</v>
       </c>
@@ -6766,16 +6812,16 @@
       <c r="T7" s="11">
         <v>-95.217492761043786</v>
       </c>
-      <c r="W7" s="55" t="s">
+      <c r="W7" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="X7" s="56"/>
-      <c r="Y7" s="56"/>
-      <c r="Z7" s="56"/>
-      <c r="AA7" s="56"/>
-      <c r="AB7" s="57"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45"/>
+      <c r="AA7" s="45"/>
+      <c r="AB7" s="46"/>
     </row>
-    <row r="8" spans="3:28" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="41" t="s">
         <v>50</v>
       </c>
@@ -6798,22 +6844,22 @@
       <c r="T8" s="11">
         <v>-93.884580470502357</v>
       </c>
-      <c r="W8" s="58" t="s">
+      <c r="W8" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="X8" s="60" t="s">
+      <c r="X8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="60" t="s">
+      <c r="Y8" s="43"/>
+      <c r="Z8" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="61"/>
+      <c r="AA8" s="43"/>
       <c r="AB8" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="3:28" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Q9" s="14">
         <v>9970</v>
       </c>
@@ -6826,20 +6872,20 @@
       <c r="T9" s="11">
         <v>-90.796195255371188</v>
       </c>
-      <c r="W9" s="59"/>
-      <c r="X9" s="60" t="s">
+      <c r="W9" s="63"/>
+      <c r="X9" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="60" t="s">
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="AA9" s="61"/>
+      <c r="AA9" s="43"/>
       <c r="AB9" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="3:28" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Q10" s="13" t="s">
         <v>14</v>
       </c>
@@ -6855,20 +6901,20 @@
       <c r="W10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="X10" s="42">
+      <c r="X10" s="49">
         <v>4.71</v>
       </c>
-      <c r="Y10" s="43"/>
-      <c r="Z10" s="46">
+      <c r="Y10" s="50"/>
+      <c r="Z10" s="53">
         <v>3.17</v>
       </c>
-      <c r="AA10" s="47"/>
+      <c r="AA10" s="54"/>
       <c r="AB10" s="11">
         <f>X10/Z10</f>
         <v>1.4858044164037856</v>
       </c>
     </row>
-    <row r="11" spans="3:28" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Q11" s="4" t="s">
         <v>15</v>
       </c>
@@ -6884,28 +6930,20 @@
       <c r="W11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="45"/>
-      <c r="Z11" s="48">
+      <c r="X11" s="51"/>
+      <c r="Y11" s="52"/>
+      <c r="Z11" s="55">
         <v>3.6</v>
       </c>
-      <c r="AA11" s="49"/>
+      <c r="AA11" s="56"/>
       <c r="AB11" s="6">
         <f>X10/Z11</f>
         <v>1.3083333333333333</v>
       </c>
     </row>
-    <row r="12" spans="3:28" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="3:28" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="W3:AB3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="X10:Y11"/>
     <mergeCell ref="Z10:AA10"/>
     <mergeCell ref="Z11:AA11"/>
@@ -6918,6 +6956,14 @@
     <mergeCell ref="Z8:AA8"/>
     <mergeCell ref="X9:Y9"/>
     <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="W3:AB3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6928,17 +6974,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EE3519-B4D8-42E5-A4D3-DAE0E3976C95}">
   <dimension ref="C2:DB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CG9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="CC5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="CM5" activeCellId="1" sqref="CM3:CS3 CM5:CS5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="26" max="26" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:106" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:106" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>38</v>
       </c>
@@ -6955,7 +7001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="3:106" ht="19.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:106" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="15" t="s">
         <v>29</v>
       </c>
@@ -7227,7 +7273,7 @@
       <c r="DA3" s="18"/>
       <c r="DB3" s="19"/>
     </row>
-    <row r="4" spans="3:106" ht="19.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:106" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="20" t="s">
         <v>30</v>
       </c>
@@ -7499,7 +7545,7 @@
       <c r="DA4" s="23"/>
       <c r="DB4" s="24"/>
     </row>
-    <row r="5" spans="3:106" ht="19.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:106" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="25" t="s">
         <v>32</v>
       </c>
@@ -7771,7 +7817,7 @@
       <c r="DA5" s="28"/>
       <c r="DB5" s="29"/>
     </row>
-    <row r="6" spans="3:106" ht="19.05" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:106" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="25" t="s">
         <v>33</v>
       </c>
@@ -8048,7 +8094,7 @@
       <c r="DA6" s="28"/>
       <c r="DB6" s="29"/>
     </row>
-    <row r="7" spans="3:106" ht="16.3" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:106" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="25" t="s">
         <v>35</v>
       </c>
@@ -8325,7 +8371,7 @@
       <c r="DA7" s="28"/>
       <c r="DB7" s="29"/>
     </row>
-    <row r="8" spans="3:106" ht="18.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:106" ht="18.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="64" t="s">
         <v>49</v>
       </c>
@@ -8427,8 +8473,8 @@
       <c r="DA8" s="65"/>
       <c r="DB8" s="66"/>
     </row>
-    <row r="9" spans="3:106" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="3:106" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:106" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="3:106" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AQ14" s="35"/>
       <c r="AR14" s="36"/>
       <c r="AS14" s="32"/>
@@ -8448,7 +8494,7 @@
       <c r="BG14" s="32"/>
       <c r="BH14" s="32"/>
     </row>
-    <row r="15" spans="3:106" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:106" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AQ15" s="35"/>
       <c r="AR15" s="37"/>
       <c r="AS15" s="32"/>
@@ -8468,7 +8514,7 @@
       <c r="BG15" s="32"/>
       <c r="BH15" s="32"/>
     </row>
-    <row r="16" spans="3:106" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:106" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AQ16" s="36"/>
       <c r="AR16" s="36"/>
       <c r="AS16" s="32"/>
@@ -8488,7 +8534,7 @@
       <c r="BG16" s="32"/>
       <c r="BH16" s="32"/>
     </row>
-    <row r="17" spans="43:60" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="17" spans="43:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AQ17" s="35"/>
       <c r="AR17" s="36"/>
       <c r="AS17" s="32"/>
@@ -8508,13 +8554,13 @@
       <c r="BG17" s="32"/>
       <c r="BH17" s="32"/>
     </row>
-    <row r="18" spans="43:60" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="18" spans="43:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AQ18" s="35"/>
       <c r="AR18" s="36"/>
       <c r="AS18" s="32"/>
       <c r="AT18" s="32"/>
     </row>
-    <row r="19" spans="43:60" ht="15.65" x14ac:dyDescent="0.25">
+    <row r="19" spans="43:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AQ19" s="38"/>
       <c r="AR19" s="38"/>
       <c r="AS19" s="38"/>

</xml_diff>